<commit_message>
Updated datasets and added download link.
</commit_message>
<xml_diff>
--- a/resources/LINCS Datasets.xlsx
+++ b/resources/LINCS Datasets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17860" yWindow="460" windowWidth="20540" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="2" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9146" uniqueCount="5622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9146" uniqueCount="5623">
   <si>
     <t>LDS-1223</t>
   </si>
@@ -17163,16 +17163,19 @@
   <si>
     <t>https://martip03.u.hpc.mssm.edu/index.php?login=1</t>
   </si>
+  <si>
+    <t>MS/MS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm"/>
-    <numFmt numFmtId="168" formatCode="#,###"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm"/>
+    <numFmt numFmtId="167" formatCode="#,###"/>
   </numFmts>
   <fonts count="46" x14ac:knownFonts="1">
     <font>
@@ -18987,7 +18990,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -19291,19 +19294,19 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -19459,7 +19462,7 @@
     <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -19474,13 +19477,13 @@
     <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -19511,6 +19514,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="45" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -21248,8 +21254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0.5"/>
@@ -22996,8 +23002,8 @@
       <c r="D41" s="168" t="s">
         <v>100</v>
       </c>
-      <c r="E41" s="170" t="s">
-        <v>239</v>
+      <c r="E41" s="201" t="s">
+        <v>100</v>
       </c>
       <c r="F41" s="168" t="s">
         <v>239</v>
@@ -23036,8 +23042,8 @@
       <c r="D42" s="168" t="s">
         <v>100</v>
       </c>
-      <c r="E42" s="170" t="s">
-        <v>239</v>
+      <c r="E42" s="201" t="s">
+        <v>100</v>
       </c>
       <c r="F42" s="168" t="s">
         <v>239</v>
@@ -23795,7 +23801,7 @@
         <v>5557</v>
       </c>
       <c r="C60" s="174" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="D60" s="174" t="s">
         <v>101</v>
@@ -23833,13 +23839,13 @@
         <v>5557</v>
       </c>
       <c r="C61" s="168" t="s">
-        <v>219</v>
+        <v>123</v>
       </c>
       <c r="D61" s="168" t="s">
         <v>100</v>
       </c>
-      <c r="E61" s="170" t="s">
-        <v>239</v>
+      <c r="E61" s="201" t="s">
+        <v>100</v>
       </c>
       <c r="F61" s="168" t="s">
         <v>239</v>
@@ -23871,13 +23877,13 @@
         <v>93</v>
       </c>
       <c r="C62" s="168" t="s">
-        <v>219</v>
+        <v>123</v>
       </c>
       <c r="D62" s="170" t="s">
         <v>239</v>
       </c>
-      <c r="E62" s="170" t="s">
-        <v>239</v>
+      <c r="E62" s="201" t="s">
+        <v>5622</v>
       </c>
       <c r="F62" s="168" t="s">
         <v>239</v>

</xml_diff>